<commit_message>
snad už konečná úprava testů
</commit_message>
<xml_diff>
--- a/K odevzdání/4. iterace/Testování/Testovací scénář - rezervace stolů.xlsx
+++ b/K odevzdání/4. iterace/Testování/Testovací scénář - rezervace stolů.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="9" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="7" r:id="rId9"/>
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
   </sheets>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="69">
   <si>
     <t>Název:</t>
   </si>
@@ -140,9 +140,6 @@
     <t xml:space="preserve">3.Zadám nesprávné údaje do kolonky data - Jméno: Tomáš Marný, Datum: XX.11.2020, Hodina: 12, Počet osob: 5, Stůl: 1 </t>
   </si>
   <si>
-    <t>1.Upozornění od systému, že formát data je špatný</t>
-  </si>
-  <si>
     <t>2.Neuložení rezervace</t>
   </si>
   <si>
@@ -158,18 +155,9 @@
     <t xml:space="preserve">3.Zadám nesprávné údaje do kolonky data - Jméno: Tomáš Marný, Datum: 1,11,2020, Hodina: 12, Počet osob: 5, Stůl: 1 </t>
   </si>
   <si>
-    <t>3.Neuložení rezervace</t>
-  </si>
-  <si>
-    <t>2.Vypsání správného formátu</t>
-  </si>
-  <si>
     <t>Poznámky:</t>
   </si>
   <si>
-    <t>Systém požaduje podle nápovědy formát DD.MM.RRRR, ale přijme i formát D.M.RRRR</t>
-  </si>
-  <si>
     <t>5.</t>
   </si>
   <si>
@@ -182,15 +170,9 @@
     <t>Ověření, zda systém kontroluje správně zadaný čas při zadávání rezervace</t>
   </si>
   <si>
-    <t>1.Upozornění od systému, že zadaná hodina není číslo</t>
-  </si>
-  <si>
     <t>8.</t>
   </si>
   <si>
-    <t>1.Upozornění od systému, že zadaná hodina neexistuje</t>
-  </si>
-  <si>
     <t>9.</t>
   </si>
   <si>
@@ -209,18 +191,12 @@
     <t xml:space="preserve">3.Zadám údaje - Jméno: Tomáš Marný, Datum: 01.01.2014, Hodina: 13, Počet osob: 5, Stůl: XX </t>
   </si>
   <si>
-    <t>1.Vypsání chybové hlášky, že zadaný zadané číslo stolu není číslo</t>
-  </si>
-  <si>
     <t>10.</t>
   </si>
   <si>
     <t xml:space="preserve">3.Zadám údaje - Jméno: Tomáš Marný, Datum: 01.01.2014, Hodina: 13, Počet osob: XX, Stůl: 1 </t>
   </si>
   <si>
-    <t>1.Vypsání chybové hlášky, že zadaný zadaný počet osob není číslo</t>
-  </si>
-  <si>
     <t>Ověření, zda systém kontroluje správně zadaný počet osob při zadávání rezervace</t>
   </si>
   <si>
@@ -234,6 +210,27 @@
   </si>
   <si>
     <t>?? - Systém dovoluje přidávat časy jen v hodinách (např.: 19), při jinak zadaném formátu ani neudává, jaký od uživatele požaduje</t>
+  </si>
+  <si>
+    <t>1.Upozornění od systému, že formát data je špatný-"Zadávejte datum ve tvaru XX.XX.XXXX"</t>
+  </si>
+  <si>
+    <t>1.Upozornění od systému, že zadaná hodina není číslo - "Chybně zadaná hodina" a zčervenání kolonky hodiny</t>
+  </si>
+  <si>
+    <t>1.Upozornění od systému, že formát data je špatný-"Zadávejte datum ve tvaru XX.XX.XXXX" a  a zčervenání kolonky data</t>
+  </si>
+  <si>
+    <t>Systém požaduje podle nápovědy formát XX.XX.XXXX, ale přijme i formát X.X.XXXX  a zčervenání kolonky data</t>
+  </si>
+  <si>
+    <t>1.Upozornění od systému, že zadaná hodina neexistuje - "Den má pouze 24 hodin"  a zčervenání kolonky času</t>
+  </si>
+  <si>
+    <t>1.Vypsání chybové hlášky, že zadané číslo stolu není číslo - "Chybně zadané číslo stolu"  a zčervenání kolonky čísla stolu</t>
+  </si>
+  <si>
+    <t>1.Vypsání chybové hlášky, že zadaný zadaný počet osob není číslo - "Chybně zadaný počet osob"  a zčervenání kolonky počtu osob</t>
   </si>
 </sst>
 </file>
@@ -665,7 +662,7 @@
   <dimension ref="A2:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +673,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -710,7 +707,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -723,7 +720,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,19 +741,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="82.28515625" customWidth="1"/>
+    <col min="2" max="2" width="114.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -764,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +787,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -873,7 +870,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -881,7 +878,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1086,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1097,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1108,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,12 +1144,12 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1171,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1182,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1193,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,7 +1216,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1232,32 +1229,27 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1269,21 +1261,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="105" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="114.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1291,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1299,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1317,7 +1309,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1330,20 +1322,15 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B13" t="s">
-        <v>9</v>
+      <c r="B12" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1357,7 +1344,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1355,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1384,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1402,7 +1389,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1415,12 +1402,12 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,21 +1426,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="114.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="105" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1461,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1469,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1487,7 +1474,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,15 +1487,20 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>69</v>
+      <c r="B13" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>